<commit_message>
Added files for analysis
</commit_message>
<xml_diff>
--- a/4B_metadata/4B_metadata_15Mar23.xlsx
+++ b/4B_metadata/4B_metadata_15Mar23.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/criseldabautista/Documents/GitHub/MADDOG_CTB/4B_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C172E36-E725-764A-B45E-36D18F1AB3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A92094-CB51-FE48-9A6D-0B800C1FDDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8560" yWindow="1980" windowWidth="26840" windowHeight="15060" xr2:uid="{6A2EE62B-E20A-784B-BAEE-4AF5B2207D62}"/>
+    <workbookView xWindow="1960" yWindow="1960" windowWidth="26840" windowHeight="15060" xr2:uid="{6A2EE62B-E20A-784B-BAEE-4AF5B2207D62}"/>
   </bookViews>
   <sheets>
-    <sheet name="MADDOG_metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="RABV_GLUE" sheetId="2" r:id="rId2"/>
+    <sheet name="metadata_4B_prov" sheetId="3" r:id="rId1"/>
+    <sheet name="MADDOG_metadata" sheetId="1" r:id="rId2"/>
+    <sheet name="RABV_GLUE" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">RABV_GLUE!$A$2:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RABV_GLUE!$A$2:$K$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -265,6 +266,135 @@
   </si>
   <si>
     <t>KX148259</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>lineage</t>
+  </si>
+  <si>
+    <t>Municipality</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Asian SEA4_A1.2</t>
+  </si>
+  <si>
+    <t>Lipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batangas </t>
+  </si>
+  <si>
+    <t>Canis familiaris</t>
+  </si>
+  <si>
+    <t>Asian SEA4_B1</t>
+  </si>
+  <si>
+    <t>General Trias</t>
+  </si>
+  <si>
+    <t>Cavite</t>
+  </si>
+  <si>
+    <t>Asian SEA4_A1.2.1</t>
+  </si>
+  <si>
+    <t>Lucena City</t>
+  </si>
+  <si>
+    <t>Quezon</t>
+  </si>
+  <si>
+    <t>Batangas City</t>
+  </si>
+  <si>
+    <t>Tayabas</t>
+  </si>
+  <si>
+    <t>Asian SEA4_B1.1.1</t>
+  </si>
+  <si>
+    <t>Calapan </t>
+  </si>
+  <si>
+    <t>Oriental Mindoro</t>
+  </si>
+  <si>
+    <t>Victoria </t>
+  </si>
+  <si>
+    <t>Puerto Galera</t>
+  </si>
+  <si>
+    <t>Baco</t>
+  </si>
+  <si>
+    <t>Asian SEA4_B1.1</t>
+  </si>
+  <si>
+    <t>Mansalay</t>
+  </si>
+  <si>
+    <t>Bongabong</t>
+  </si>
+  <si>
+    <t>Gloria</t>
+  </si>
+  <si>
+    <t>Pinamalayan</t>
+  </si>
+  <si>
+    <t>Pola</t>
+  </si>
+  <si>
+    <t>Roxas</t>
+  </si>
+  <si>
+    <t>Alcantara</t>
+  </si>
+  <si>
+    <t>Romblon</t>
+  </si>
+  <si>
+    <t>Odiongan</t>
+  </si>
+  <si>
+    <t>Santa Maria</t>
+  </si>
+  <si>
+    <t>San Agustin</t>
+  </si>
+  <si>
+    <t>San Andres</t>
+  </si>
+  <si>
+    <t>Calintaan</t>
+  </si>
+  <si>
+    <t>Occidental Mindoro</t>
+  </si>
+  <si>
+    <t>Homo sapiens</t>
+  </si>
+  <si>
+    <t>19/12/20223</t>
   </si>
 </sst>
 </file>
@@ -313,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -322,6 +452,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,10 +766,1568 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445BFD04-0A65-2744-A6E1-D634293E2516}">
+  <dimension ref="A1:I53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2022</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2">
+        <v>13.94086577</v>
+      </c>
+      <c r="G2">
+        <v>121.1746864</v>
+      </c>
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="6">
+        <v>44586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3">
+        <v>14.329666189999999</v>
+      </c>
+      <c r="G3">
+        <v>120.8999068</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="6">
+        <v>44598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>2022</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4">
+        <v>13.938347540000001</v>
+      </c>
+      <c r="G4">
+        <v>121.61535929999999</v>
+      </c>
+      <c r="H4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="6">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2022</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5">
+        <v>13.7207195</v>
+      </c>
+      <c r="G5">
+        <v>121.103796</v>
+      </c>
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="6">
+        <v>44571</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2022</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6">
+        <v>14.04055469</v>
+      </c>
+      <c r="G6">
+        <v>121.6122459</v>
+      </c>
+      <c r="H6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="6">
+        <v>44583</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>2021</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7">
+        <v>13.331785119999999</v>
+      </c>
+      <c r="G7">
+        <v>121.1780294</v>
+      </c>
+      <c r="H7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="6">
+        <v>44222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2021</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8">
+        <v>13.14368391</v>
+      </c>
+      <c r="G8">
+        <v>121.2438544</v>
+      </c>
+      <c r="H8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="6">
+        <v>44236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>2021</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9">
+        <v>13.392176409999999</v>
+      </c>
+      <c r="G9">
+        <v>120.8953101</v>
+      </c>
+      <c r="H9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="6">
+        <v>44265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2021</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10">
+        <v>13.392176409999999</v>
+      </c>
+      <c r="G10">
+        <v>120.8953101</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="6">
+        <v>44260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2021</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11">
+        <v>13.392176409999999</v>
+      </c>
+      <c r="G11">
+        <v>120.8953101</v>
+      </c>
+      <c r="H11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="6">
+        <v>44298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2021</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12">
+        <v>13.29039427</v>
+      </c>
+      <c r="G12">
+        <v>121.06683700000001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="6">
+        <v>44300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>2021</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13">
+        <v>13.331785119999999</v>
+      </c>
+      <c r="G13">
+        <v>121.1780294</v>
+      </c>
+      <c r="H13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="6">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>2021</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14">
+        <v>13.392176409999999</v>
+      </c>
+      <c r="G14">
+        <v>120.8953101</v>
+      </c>
+      <c r="H14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="6">
+        <v>44344</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2022</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15">
+        <v>13.29039427</v>
+      </c>
+      <c r="G15">
+        <v>121.06683700000001</v>
+      </c>
+      <c r="H15" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="6">
+        <v>44608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16">
+        <v>13.29039427</v>
+      </c>
+      <c r="G16">
+        <v>121.06683700000001</v>
+      </c>
+      <c r="H16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="6">
+        <v>44575</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>2022</v>
+      </c>
+      <c r="C17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17">
+        <v>12.548369689999999</v>
+      </c>
+      <c r="G17">
+        <v>121.34821340000001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="6">
+        <v>44673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>2022</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18">
+        <v>13.392176409999999</v>
+      </c>
+      <c r="G18">
+        <v>120.8953101</v>
+      </c>
+      <c r="H18" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="6">
+        <v>44566</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>2022</v>
+      </c>
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19">
+        <v>12.71623574</v>
+      </c>
+      <c r="G19">
+        <v>121.38623029999999</v>
+      </c>
+      <c r="H19" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="6">
+        <v>44679</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2022</v>
+      </c>
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20">
+        <v>12.92166054</v>
+      </c>
+      <c r="G20">
+        <v>121.3754507</v>
+      </c>
+      <c r="H20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="6">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>2022</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21">
+        <v>12.548369689999999</v>
+      </c>
+      <c r="G21">
+        <v>121.34821340000001</v>
+      </c>
+      <c r="H21" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="6">
+        <v>44700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>2022</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22">
+        <v>13.02301767</v>
+      </c>
+      <c r="G22">
+        <v>121.4031803</v>
+      </c>
+      <c r="H22" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="6">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>2022</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23">
+        <v>13.29039427</v>
+      </c>
+      <c r="G23">
+        <v>121.06683700000001</v>
+      </c>
+      <c r="H23" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" s="6">
+        <v>44769</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>2022</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24">
+        <v>13.29039427</v>
+      </c>
+      <c r="G24">
+        <v>121.06683700000001</v>
+      </c>
+      <c r="H24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="6">
+        <v>44785</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>2022</v>
+      </c>
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25">
+        <v>13.13990357</v>
+      </c>
+      <c r="G25">
+        <v>121.44494779999999</v>
+      </c>
+      <c r="H25" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" s="6">
+        <v>44791</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>2022</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26">
+        <v>12.617370510000001</v>
+      </c>
+      <c r="G26">
+        <v>121.4554967</v>
+      </c>
+      <c r="H26" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" s="6">
+        <v>44859</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <v>2022</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27">
+        <v>12.29784708</v>
+      </c>
+      <c r="G27">
+        <v>122.054934</v>
+      </c>
+      <c r="H27" t="s">
+        <v>86</v>
+      </c>
+      <c r="I27" s="6">
+        <v>44835</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>2022</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28">
+        <v>12.29784708</v>
+      </c>
+      <c r="G28">
+        <v>122.054934</v>
+      </c>
+      <c r="H28" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="6">
+        <v>44855</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2022</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29">
+        <v>12.548369689999999</v>
+      </c>
+      <c r="G29">
+        <v>121.34821340000001</v>
+      </c>
+      <c r="H29" t="s">
+        <v>86</v>
+      </c>
+      <c r="I29" s="6">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>2022</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30">
+        <v>12.39865996</v>
+      </c>
+      <c r="G30">
+        <v>122.01777010000001</v>
+      </c>
+      <c r="H30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I30" s="6">
+        <v>44889</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <v>2022</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31">
+        <v>12.29784708</v>
+      </c>
+      <c r="G31">
+        <v>122.054934</v>
+      </c>
+      <c r="H31" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" s="6">
+        <v>44891</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>2022</v>
+      </c>
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32">
+        <v>12.39865996</v>
+      </c>
+      <c r="G32">
+        <v>122.01777010000001</v>
+      </c>
+      <c r="H32" t="s">
+        <v>86</v>
+      </c>
+      <c r="I32" s="6">
+        <v>44906</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>2022</v>
+      </c>
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33">
+        <v>12.40310216</v>
+      </c>
+      <c r="G33">
+        <v>122.0836566</v>
+      </c>
+      <c r="H33" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" s="6">
+        <v>44907</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>2023</v>
+      </c>
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34">
+        <v>12.40310216</v>
+      </c>
+      <c r="G34">
+        <v>122.0836566</v>
+      </c>
+      <c r="H34" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" s="6">
+        <v>44946</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>2023</v>
+      </c>
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35">
+        <v>12.39865996</v>
+      </c>
+      <c r="G35">
+        <v>122.01777010000001</v>
+      </c>
+      <c r="H35" t="s">
+        <v>86</v>
+      </c>
+      <c r="I35" s="6">
+        <v>44939</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>2023</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36">
+        <v>12.554035519999999</v>
+      </c>
+      <c r="G36">
+        <v>122.11240479999999</v>
+      </c>
+      <c r="H36" t="s">
+        <v>86</v>
+      </c>
+      <c r="I36" s="6">
+        <v>44948</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>2023</v>
+      </c>
+      <c r="C37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37">
+        <v>12.554035519999999</v>
+      </c>
+      <c r="G37">
+        <v>122.11240479999999</v>
+      </c>
+      <c r="H37" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37" s="6">
+        <v>44957</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>2023</v>
+      </c>
+      <c r="C38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" t="s">
+        <v>112</v>
+      </c>
+      <c r="E38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38">
+        <v>12.554035519999999</v>
+      </c>
+      <c r="G38">
+        <v>122.11240479999999</v>
+      </c>
+      <c r="H38" t="s">
+        <v>86</v>
+      </c>
+      <c r="I38" s="6">
+        <v>44956</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>2023</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39">
+        <v>12.40310216</v>
+      </c>
+      <c r="G39">
+        <v>122.0836566</v>
+      </c>
+      <c r="H39" t="s">
+        <v>86</v>
+      </c>
+      <c r="I39" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>2023</v>
+      </c>
+      <c r="C40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40">
+        <v>12.40310216</v>
+      </c>
+      <c r="G40">
+        <v>122.0836566</v>
+      </c>
+      <c r="H40" t="s">
+        <v>86</v>
+      </c>
+      <c r="I40" s="6">
+        <v>44964</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>2023</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41">
+        <v>12.53642104</v>
+      </c>
+      <c r="G41">
+        <v>122.0469478</v>
+      </c>
+      <c r="H41" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" s="6">
+        <v>44964</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>2023</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42">
+        <v>12.39865996</v>
+      </c>
+      <c r="G42">
+        <v>122.01777010000001</v>
+      </c>
+      <c r="H42" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" s="6">
+        <v>44966</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>2023</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F43">
+        <v>12.39865996</v>
+      </c>
+      <c r="G43">
+        <v>122.01777010000001</v>
+      </c>
+      <c r="H43" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" s="6">
+        <v>44973</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>2023</v>
+      </c>
+      <c r="C44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44">
+        <v>12.39865996</v>
+      </c>
+      <c r="G44">
+        <v>122.01777010000001</v>
+      </c>
+      <c r="H44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" s="6">
+        <v>44985</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>2023</v>
+      </c>
+      <c r="C45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" t="s">
+        <v>109</v>
+      </c>
+      <c r="F45">
+        <v>12.39865996</v>
+      </c>
+      <c r="G45">
+        <v>122.01777010000001</v>
+      </c>
+      <c r="H45" t="s">
+        <v>86</v>
+      </c>
+      <c r="I45" s="6">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>2023</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" t="s">
+        <v>112</v>
+      </c>
+      <c r="E46" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46">
+        <v>12.554035519999999</v>
+      </c>
+      <c r="G46">
+        <v>122.11240479999999</v>
+      </c>
+      <c r="H46" t="s">
+        <v>86</v>
+      </c>
+      <c r="I46" s="6">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47">
+        <v>2022</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" t="s">
+        <v>114</v>
+      </c>
+      <c r="E47" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47">
+        <v>12.592177059999999</v>
+      </c>
+      <c r="G47">
+        <v>121.08265900000001</v>
+      </c>
+      <c r="H47" t="s">
+        <v>86</v>
+      </c>
+      <c r="I47" s="6">
+        <v>44596</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>2022</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" t="s">
+        <v>97</v>
+      </c>
+      <c r="F48">
+        <v>13.29039427</v>
+      </c>
+      <c r="G48">
+        <v>121.06683700000001</v>
+      </c>
+      <c r="H48" t="s">
+        <v>86</v>
+      </c>
+      <c r="I48" s="6">
+        <v>44601</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49">
+        <v>2022</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49">
+        <v>12.71623574</v>
+      </c>
+      <c r="G49">
+        <v>121.38623029999999</v>
+      </c>
+      <c r="H49" t="s">
+        <v>86</v>
+      </c>
+      <c r="I49" s="6">
+        <v>44601</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>2023</v>
+      </c>
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50">
+        <v>12.40310216</v>
+      </c>
+      <c r="G50">
+        <v>122.0836566</v>
+      </c>
+      <c r="H50" t="s">
+        <v>116</v>
+      </c>
+      <c r="I50" s="6">
+        <v>44960</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51">
+        <v>2023</v>
+      </c>
+      <c r="C51" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51">
+        <v>12.40310216</v>
+      </c>
+      <c r="G51">
+        <v>122.0836566</v>
+      </c>
+      <c r="H51" t="s">
+        <v>116</v>
+      </c>
+      <c r="I51" s="6">
+        <v>44960</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>2022</v>
+      </c>
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52">
+        <v>12.40310216</v>
+      </c>
+      <c r="G52">
+        <v>122.0836566</v>
+      </c>
+      <c r="H52" t="s">
+        <v>86</v>
+      </c>
+      <c r="I52" s="6">
+        <v>44886</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53">
+        <v>2022</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" t="s">
+        <v>109</v>
+      </c>
+      <c r="F53">
+        <v>12.554035519999999</v>
+      </c>
+      <c r="G53">
+        <v>122.11240479999999</v>
+      </c>
+      <c r="H53" t="s">
+        <v>86</v>
+      </c>
+      <c r="I53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE02-173A-BA42-833A-BB895E89D1AF}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1450,7 +3139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25345CD-A764-C443-858F-2814D0CE40A7}">
   <dimension ref="A1:K54"/>
   <sheetViews>
@@ -1539,7 +3228,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K3" s="3">
-        <f>AVERAGE(F3:J3)</f>
+        <f t="shared" ref="K3:K34" si="0">AVERAGE(F3:J3)</f>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -1575,7 +3264,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K4" s="3">
-        <f>AVERAGE(F4:J4)</f>
+        <f t="shared" si="0"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -1611,7 +3300,7 @@
         <v>0.93530000000000002</v>
       </c>
       <c r="K5" s="3">
-        <f>AVERAGE(F5:J5)</f>
+        <f t="shared" si="0"/>
         <v>0.94114000000000009</v>
       </c>
     </row>
@@ -1647,7 +3336,7 @@
         <v>0.91720000000000002</v>
       </c>
       <c r="K6" s="3">
-        <f>AVERAGE(F6:J6)</f>
+        <f t="shared" si="0"/>
         <v>0.95690000000000008</v>
       </c>
     </row>
@@ -1683,7 +3372,7 @@
         <v>0.96160000000000001</v>
       </c>
       <c r="K7" s="3">
-        <f>AVERAGE(F7:J7)</f>
+        <f t="shared" si="0"/>
         <v>0.99231999999999998</v>
       </c>
     </row>
@@ -1719,7 +3408,7 @@
         <v>0.9617</v>
       </c>
       <c r="K8" s="3">
-        <f>AVERAGE(F8:J8)</f>
+        <f t="shared" si="0"/>
         <v>0.99234000000000011</v>
       </c>
     </row>
@@ -1755,7 +3444,7 @@
         <v>0.9617</v>
       </c>
       <c r="K9" s="3">
-        <f>AVERAGE(F9:J9)</f>
+        <f t="shared" si="0"/>
         <v>0.99234000000000011</v>
       </c>
     </row>
@@ -1791,7 +3480,7 @@
         <v>0.96619999999999995</v>
       </c>
       <c r="K10" s="3">
-        <f>AVERAGE(F10:J10)</f>
+        <f t="shared" si="0"/>
         <v>0.9932399999999999</v>
       </c>
     </row>
@@ -1827,7 +3516,7 @@
         <v>0.9667</v>
       </c>
       <c r="K11" s="3">
-        <f>AVERAGE(F11:J11)</f>
+        <f t="shared" si="0"/>
         <v>0.99334000000000011</v>
       </c>
     </row>
@@ -1863,7 +3552,7 @@
         <v>0.99880000000000002</v>
       </c>
       <c r="K12" s="3">
-        <f>AVERAGE(F12:J12)</f>
+        <f t="shared" si="0"/>
         <v>0.99975999999999998</v>
       </c>
     </row>
@@ -1899,7 +3588,7 @@
         <v>0.9617</v>
       </c>
       <c r="K13" s="3">
-        <f>AVERAGE(F13:J13)</f>
+        <f t="shared" si="0"/>
         <v>0.99234000000000011</v>
       </c>
     </row>
@@ -1935,7 +3624,7 @@
         <v>0.93510000000000004</v>
       </c>
       <c r="K14" s="3">
-        <f>AVERAGE(F14:J14)</f>
+        <f t="shared" si="0"/>
         <v>0.98702000000000001</v>
       </c>
     </row>
@@ -1971,7 +3660,7 @@
         <v>0.96</v>
       </c>
       <c r="K15" s="3">
-        <f>AVERAGE(F15:J15)</f>
+        <f t="shared" si="0"/>
         <v>0.99199999999999999</v>
       </c>
     </row>
@@ -2007,7 +3696,7 @@
         <v>0.9617</v>
       </c>
       <c r="K16" s="3">
-        <f>AVERAGE(F16:J16)</f>
+        <f t="shared" si="0"/>
         <v>0.9658000000000001</v>
       </c>
     </row>
@@ -2043,7 +3732,7 @@
         <v>0.9617</v>
       </c>
       <c r="K17" s="3">
-        <f>AVERAGE(F17:J17)</f>
+        <f t="shared" si="0"/>
         <v>0.99234000000000011</v>
       </c>
     </row>
@@ -2079,7 +3768,7 @@
         <v>0.93510000000000004</v>
       </c>
       <c r="K18" s="3">
-        <f>AVERAGE(F18:J18)</f>
+        <f t="shared" si="0"/>
         <v>0.98702000000000001</v>
       </c>
     </row>
@@ -2115,7 +3804,7 @@
         <v>0.99880000000000002</v>
       </c>
       <c r="K19" s="3">
-        <f>AVERAGE(F19:J19)</f>
+        <f t="shared" si="0"/>
         <v>0.99975999999999998</v>
       </c>
     </row>
@@ -2151,7 +3840,7 @@
         <v>0.93510000000000004</v>
       </c>
       <c r="K20" s="3">
-        <f>AVERAGE(F20:J20)</f>
+        <f t="shared" si="0"/>
         <v>0.98702000000000001</v>
       </c>
     </row>
@@ -2187,7 +3876,7 @@
         <v>0.90290000000000004</v>
       </c>
       <c r="K21" s="3">
-        <f>AVERAGE(F21:J21)</f>
+        <f t="shared" si="0"/>
         <v>0.95404</v>
       </c>
     </row>
@@ -2223,7 +3912,7 @@
         <v>0.93510000000000004</v>
       </c>
       <c r="K22" s="3">
-        <f>AVERAGE(F22:J22)</f>
+        <f t="shared" si="0"/>
         <v>0.96048000000000011</v>
       </c>
     </row>
@@ -2259,7 +3948,7 @@
         <v>0.90280000000000005</v>
       </c>
       <c r="K23" s="3">
-        <f>AVERAGE(F23:J23)</f>
+        <f t="shared" si="0"/>
         <v>0.95402000000000009</v>
       </c>
     </row>
@@ -2295,7 +3984,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K24" s="3">
-        <f>AVERAGE(F24:J24)</f>
+        <f t="shared" si="0"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2331,7 +4020,7 @@
         <v>0.68830000000000002</v>
       </c>
       <c r="K25" s="3">
-        <f>AVERAGE(F25:J25)</f>
+        <f t="shared" si="0"/>
         <v>0.73815999999999993</v>
       </c>
     </row>
@@ -2367,7 +4056,7 @@
         <v>0.95289999999999997</v>
       </c>
       <c r="K26" s="3">
-        <f>AVERAGE(F26:J26)</f>
+        <f t="shared" si="0"/>
         <v>0.99057999999999991</v>
       </c>
     </row>
@@ -2403,7 +4092,7 @@
         <v>0.93510000000000004</v>
       </c>
       <c r="K27" s="3">
-        <f>AVERAGE(F27:J27)</f>
+        <f t="shared" si="0"/>
         <v>0.98702000000000001</v>
       </c>
     </row>
@@ -2439,7 +4128,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K28" s="3">
-        <f>AVERAGE(F28:J28)</f>
+        <f t="shared" si="0"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2475,7 +4164,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K29" s="3">
-        <f>AVERAGE(F29:J29)</f>
+        <f t="shared" si="0"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2511,7 +4200,7 @@
         <v>0.93510000000000004</v>
       </c>
       <c r="K30" s="3">
-        <f>AVERAGE(F30:J30)</f>
+        <f t="shared" si="0"/>
         <v>0.96048000000000011</v>
       </c>
     </row>
@@ -2547,7 +4236,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K31" s="3">
-        <f>AVERAGE(F31:J31)</f>
+        <f t="shared" si="0"/>
         <v>0.9504999999999999</v>
       </c>
     </row>
@@ -2583,7 +4272,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K32" s="3">
-        <f>AVERAGE(F32:J32)</f>
+        <f t="shared" si="0"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2619,7 +4308,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K33" s="3">
-        <f>AVERAGE(F33:J33)</f>
+        <f t="shared" si="0"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2655,7 +4344,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K34" s="3">
-        <f>AVERAGE(F34:J34)</f>
+        <f t="shared" si="0"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2691,7 +4380,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K35" s="3">
-        <f>AVERAGE(F35:J35)</f>
+        <f t="shared" ref="K35:K66" si="1">AVERAGE(F35:J35)</f>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2727,7 +4416,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K36" s="3">
-        <f>AVERAGE(F36:J36)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2763,7 +4452,7 @@
         <v>0.99860000000000004</v>
       </c>
       <c r="K37" s="3">
-        <f>AVERAGE(F37:J37)</f>
+        <f t="shared" si="1"/>
         <v>0.99971999999999994</v>
       </c>
     </row>
@@ -2799,7 +4488,7 @@
         <v>0.99860000000000004</v>
       </c>
       <c r="K38" s="3">
-        <f>AVERAGE(F38:J38)</f>
+        <f t="shared" si="1"/>
         <v>0.99971999999999994</v>
       </c>
     </row>
@@ -2835,7 +4524,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K39" s="3">
-        <f>AVERAGE(F39:J39)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2871,7 +4560,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K40" s="3">
-        <f>AVERAGE(F40:J40)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2907,7 +4596,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K41" s="3">
-        <f>AVERAGE(F41:J41)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2943,7 +4632,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K42" s="3">
-        <f>AVERAGE(F42:J42)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -2979,7 +4668,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K43" s="3">
-        <f>AVERAGE(F43:J43)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -3015,7 +4704,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K44" s="3">
-        <f>AVERAGE(F44:J44)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -3051,7 +4740,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K45" s="3">
-        <f>AVERAGE(F45:J45)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -3087,7 +4776,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K46" s="3">
-        <f>AVERAGE(F46:J46)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -3123,7 +4812,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K47" s="3">
-        <f>AVERAGE(F47:J47)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -3159,7 +4848,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K48" s="3">
-        <f>AVERAGE(F48:J48)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -3195,7 +4884,7 @@
         <v>0.9617</v>
       </c>
       <c r="K49" s="3">
-        <f>AVERAGE(F49:J49)</f>
+        <f t="shared" si="1"/>
         <v>0.9658000000000001</v>
       </c>
     </row>
@@ -3231,7 +4920,7 @@
         <v>0.9617</v>
       </c>
       <c r="K50" s="3">
-        <f>AVERAGE(F50:J50)</f>
+        <f t="shared" si="1"/>
         <v>0.99234000000000011</v>
       </c>
     </row>
@@ -3267,7 +4956,7 @@
         <v>0.22409999999999999</v>
       </c>
       <c r="K51" s="3">
-        <f>AVERAGE(F51:J51)</f>
+        <f t="shared" si="1"/>
         <v>0.34337999999999996</v>
       </c>
     </row>
@@ -3303,7 +4992,7 @@
         <v>0.8619</v>
       </c>
       <c r="K52" s="3">
-        <f>AVERAGE(F52:J52)</f>
+        <f t="shared" si="1"/>
         <v>0.92892000000000008</v>
       </c>
     </row>
@@ -3339,7 +5028,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="K53" s="3">
-        <f>AVERAGE(F53:J53)</f>
+        <f t="shared" si="1"/>
         <v>0.99439999999999995</v>
       </c>
     </row>
@@ -3375,7 +5064,7 @@
         <v>0.85750000000000004</v>
       </c>
       <c r="K54" s="3">
-        <f>AVERAGE(F54:J54)</f>
+        <f t="shared" si="1"/>
         <v>0.92803999999999998</v>
       </c>
     </row>

</xml_diff>